<commit_message>
Actualizacion cronograma de calidad
</commit_message>
<xml_diff>
--- a/Organización/Calidad/Cronograma_calidad.xlsx
+++ b/Organización/Calidad/Cronograma_calidad.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,13 +66,19 @@
     <t>Esfuerzo real</t>
   </si>
   <si>
-    <t>Fecha inicio</t>
-  </si>
-  <si>
-    <t>Fecha fin</t>
-  </si>
-  <si>
-    <t>Recurso</t>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Fecha inicio real</t>
+  </si>
+  <si>
+    <t>Fecha fin real</t>
+  </si>
+  <si>
+    <t>Fecha fin planeada</t>
+  </si>
+  <si>
+    <t>Fecha inicio planeada</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,12 +479,14 @@
     <col min="1" max="1" width="41.28515625" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -489,16 +497,22 @@
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -507,8 +521,10 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
@@ -517,8 +533,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -527,8 +545,10 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -537,8 +557,10 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -547,8 +569,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -557,8 +581,10 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -567,8 +593,10 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -577,8 +605,10 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -587,8 +617,10 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -597,8 +629,10 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -607,8 +641,10 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -617,8 +653,10 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -627,14 +665,8 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>